<commit_message>
Fixed some issues in CM that were causing warnings. Moved one of the hasInternetAddress mappings to the row were the corresponding XPath was (v.2.8.1). We've repeated the field name and XPATH info for the second row for II.2 Description (v.2.8.3).
</commit_message>
<xml_diff>
--- a/mappings/package_F06/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F06/transformation/conceptual_mappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="1054">
   <si>
     <t>Field</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>2.8.1</t>
+    <t>2.8.3</t>
   </si>
   <si>
     <r>
@@ -1444,6 +1444,9 @@
     </r>
   </si>
   <si>
+    <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY_ADDITIONAL/URL_GENERAL</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1481,9 +1484,6 @@
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
-  </si>
-  <si>
-    <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY_ADDITIONAL/URL_GENERAL</t>
   </si>
   <si>
     <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY_ADDITIONAL/URL_BUYER</t>
@@ -7474,6 +7474,10 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <color rgb="FF0000FF"/>
@@ -7487,10 +7491,6 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FFB7B7B7"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -7594,7 +7594,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7665,6 +7665,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -7764,7 +7770,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="186">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7985,16 +7991,22 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="7" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -8003,16 +8015,16 @@
     <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="10" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -8081,19 +8093,25 @@
     <xf quotePrefix="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -8272,7 +8290,7 @@
     <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="15" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -11701,6 +11719,7 @@
     <col customWidth="1" min="7" max="7" width="24.0"/>
     <col customWidth="1" min="8" max="8" width="32.88"/>
     <col customWidth="1" min="9" max="10" width="26.13"/>
+    <col customWidth="1" min="11" max="11" width="54.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12828,12 +12847,8 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="H34" s="47" t="s">
-        <v>172</v>
-      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="6"/>
@@ -12859,11 +12874,15 @@
         <v>134</v>
       </c>
       <c r="E35" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="45"/>
+      <c r="G35" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
       <c r="I35" s="45"/>
       <c r="J35" s="45"/>
       <c r="K35" s="60"/>
@@ -13608,11 +13627,17 @@
       <c r="R58" s="29"/>
     </row>
     <row r="59">
-      <c r="A59" s="76"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="76" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59" s="77" t="s">
+        <v>8</v>
+      </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="F59" s="4"/>
       <c r="G59" s="42" t="s">
         <v>282</v>
@@ -13982,7 +14007,7 @@
       <c r="H71" s="39"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
-      <c r="K71" s="77" t="s">
+      <c r="K71" s="78" t="s">
         <v>328</v>
       </c>
       <c r="L71" s="29"/>
@@ -13994,7 +14019,7 @@
       <c r="R71" s="29"/>
     </row>
     <row r="72">
-      <c r="A72" s="76"/>
+      <c r="A72" s="79"/>
       <c r="B72" s="4"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -14005,7 +14030,7 @@
       <c r="G72" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="H72" s="78" t="s">
+      <c r="H72" s="80" t="s">
         <v>331</v>
       </c>
       <c r="I72" s="6"/>
@@ -14039,7 +14064,7 @@
       <c r="G73" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="H73" s="79" t="s">
+      <c r="H73" s="81" t="s">
         <v>337</v>
       </c>
       <c r="I73" s="6"/>
@@ -14054,10 +14079,10 @@
       <c r="R73" s="29"/>
     </row>
     <row r="74">
-      <c r="A74" s="80" t="s">
+      <c r="A74" s="82" t="s">
         <v>338</v>
       </c>
-      <c r="B74" s="81" t="s">
+      <c r="B74" s="83" t="s">
         <v>339</v>
       </c>
       <c r="C74" s="53" t="s">
@@ -14073,7 +14098,7 @@
       <c r="G74" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="H74" s="82" t="s">
+      <c r="H74" s="84" t="s">
         <v>344</v>
       </c>
       <c r="I74" s="6"/>
@@ -14088,10 +14113,10 @@
       <c r="R74" s="29"/>
     </row>
     <row r="75">
-      <c r="A75" s="80" t="s">
+      <c r="A75" s="82" t="s">
         <v>345</v>
       </c>
-      <c r="B75" s="81" t="s">
+      <c r="B75" s="83" t="s">
         <v>346</v>
       </c>
       <c r="C75" s="53" t="s">
@@ -14107,7 +14132,7 @@
       <c r="G75" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="H75" s="82" t="s">
+      <c r="H75" s="84" t="s">
         <v>350</v>
       </c>
       <c r="I75" s="6"/>
@@ -14122,7 +14147,7 @@
       <c r="R75" s="29"/>
     </row>
     <row r="76">
-      <c r="A76" s="76"/>
+      <c r="A76" s="79"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -14133,7 +14158,7 @@
       <c r="G76" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="H76" s="78" t="s">
+      <c r="H76" s="80" t="s">
         <v>352</v>
       </c>
       <c r="I76" s="6"/>
@@ -14167,7 +14192,7 @@
       <c r="G77" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="H77" s="79" t="s">
+      <c r="H77" s="81" t="s">
         <v>355</v>
       </c>
       <c r="I77" s="6"/>
@@ -14182,10 +14207,10 @@
       <c r="R77" s="29"/>
     </row>
     <row r="78">
-      <c r="A78" s="80" t="s">
+      <c r="A78" s="82" t="s">
         <v>356</v>
       </c>
-      <c r="B78" s="81" t="s">
+      <c r="B78" s="83" t="s">
         <v>339</v>
       </c>
       <c r="C78" s="53" t="s">
@@ -14201,7 +14226,7 @@
       <c r="G78" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="H78" s="82" t="s">
+      <c r="H78" s="84" t="s">
         <v>344</v>
       </c>
       <c r="I78" s="6"/>
@@ -14216,10 +14241,10 @@
       <c r="R78" s="29"/>
     </row>
     <row r="79">
-      <c r="A79" s="80" t="s">
+      <c r="A79" s="82" t="s">
         <v>358</v>
       </c>
-      <c r="B79" s="81" t="s">
+      <c r="B79" s="83" t="s">
         <v>346</v>
       </c>
       <c r="C79" s="53" t="s">
@@ -14250,7 +14275,7 @@
       <c r="R79" s="29"/>
     </row>
     <row r="80">
-      <c r="A80" s="76"/>
+      <c r="A80" s="79"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -14295,7 +14320,7 @@
       <c r="G81" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="H81" s="79" t="s">
+      <c r="H81" s="81" t="s">
         <v>364</v>
       </c>
       <c r="I81" s="6"/>
@@ -14310,10 +14335,10 @@
       <c r="R81" s="29"/>
     </row>
     <row r="82">
-      <c r="A82" s="80" t="s">
+      <c r="A82" s="82" t="s">
         <v>365</v>
       </c>
-      <c r="B82" s="81" t="s">
+      <c r="B82" s="83" t="s">
         <v>346</v>
       </c>
       <c r="C82" s="53" t="s">
@@ -14402,16 +14427,16 @@
       <c r="R84" s="29"/>
     </row>
     <row r="85">
-      <c r="A85" s="83" t="s">
+      <c r="A85" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="B85" s="84" t="s">
+      <c r="B85" s="86" t="s">
         <v>370</v>
       </c>
-      <c r="C85" s="85" t="s">
+      <c r="C85" s="87" t="s">
         <v>371</v>
       </c>
-      <c r="D85" s="85" t="s">
+      <c r="D85" s="87" t="s">
         <v>370</v>
       </c>
       <c r="E85" s="53" t="s">
@@ -14487,7 +14512,7 @@
       <c r="K87" s="6"/>
     </row>
     <row r="88">
-      <c r="A88" s="86" t="s">
+      <c r="A88" s="88" t="s">
         <v>386</v>
       </c>
       <c r="B88" s="59" t="s">
@@ -14514,16 +14539,16 @@
       <c r="K88" s="6"/>
     </row>
     <row r="89">
-      <c r="A89" s="87" t="s">
+      <c r="A89" s="89" t="s">
         <v>386</v>
       </c>
-      <c r="B89" s="88" t="s">
+      <c r="B89" s="90" t="s">
         <v>387</v>
       </c>
-      <c r="C89" s="89" t="s">
+      <c r="C89" s="91" t="s">
         <v>388</v>
       </c>
-      <c r="D89" s="89" t="s">
+      <c r="D89" s="91" t="s">
         <v>389</v>
       </c>
       <c r="E89" s="53" t="s">
@@ -14541,7 +14566,7 @@
       <c r="K89" s="6"/>
     </row>
     <row r="90">
-      <c r="A90" s="86" t="s">
+      <c r="A90" s="88" t="s">
         <v>395</v>
       </c>
       <c r="B90" s="59" t="s">
@@ -14560,7 +14585,7 @@
       <c r="G90" s="53" t="s">
         <v>400</v>
       </c>
-      <c r="H90" s="90" t="s">
+      <c r="H90" s="92" t="s">
         <v>401</v>
       </c>
       <c r="I90" s="6"/>
@@ -14587,7 +14612,7 @@
       <c r="G91" s="42" t="s">
         <v>286</v>
       </c>
-      <c r="H91" s="91" t="s">
+      <c r="H91" s="93" t="s">
         <v>407</v>
       </c>
       <c r="I91" s="6"/>
@@ -14595,7 +14620,7 @@
       <c r="K91" s="6"/>
     </row>
     <row r="92">
-      <c r="A92" s="92" t="s">
+      <c r="A92" s="94" t="s">
         <v>408</v>
       </c>
       <c r="B92" s="41" t="s">
@@ -14629,7 +14654,7 @@
       <c r="K93" s="6"/>
     </row>
     <row r="94">
-      <c r="A94" s="86" t="s">
+      <c r="A94" s="88" t="s">
         <v>411</v>
       </c>
       <c r="B94" s="59" t="s">
@@ -14648,7 +14673,7 @@
       <c r="G94" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H94" s="78" t="s">
+      <c r="H94" s="80" t="s">
         <v>417</v>
       </c>
       <c r="I94" s="6"/>
@@ -14656,7 +14681,7 @@
       <c r="K94" s="6"/>
     </row>
     <row r="95">
-      <c r="A95" s="86" t="s">
+      <c r="A95" s="88" t="s">
         <v>418</v>
       </c>
       <c r="B95" s="59" t="s">
@@ -14675,7 +14700,7 @@
       <c r="G95" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H95" s="78" t="s">
+      <c r="H95" s="80" t="s">
         <v>421</v>
       </c>
       <c r="I95" s="6"/>
@@ -14683,7 +14708,7 @@
       <c r="K95" s="6"/>
     </row>
     <row r="96">
-      <c r="A96" s="86" t="s">
+      <c r="A96" s="88" t="s">
         <v>422</v>
       </c>
       <c r="B96" s="59" t="s">
@@ -14695,14 +14720,14 @@
       <c r="D96" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="E96" s="93" t="s">
+      <c r="E96" s="95" t="s">
         <v>424</v>
       </c>
       <c r="F96" s="37"/>
       <c r="G96" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H96" s="94" t="s">
+      <c r="H96" s="96" t="s">
         <v>425</v>
       </c>
       <c r="I96" s="6"/>
@@ -14710,7 +14735,7 @@
       <c r="K96" s="6"/>
     </row>
     <row r="97">
-      <c r="A97" s="86" t="s">
+      <c r="A97" s="88" t="s">
         <v>426</v>
       </c>
       <c r="B97" s="59" t="s">
@@ -14722,7 +14747,7 @@
       <c r="D97" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="E97" s="93" t="s">
+      <c r="E97" s="95" t="s">
         <v>428</v>
       </c>
       <c r="F97" s="37"/>
@@ -14737,7 +14762,7 @@
       <c r="K97" s="6"/>
     </row>
     <row r="98">
-      <c r="A98" s="86" t="s">
+      <c r="A98" s="88" t="s">
         <v>430</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -14749,14 +14774,14 @@
       <c r="D98" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="E98" s="93" t="s">
+      <c r="E98" s="95" t="s">
         <v>432</v>
       </c>
       <c r="F98" s="37"/>
       <c r="G98" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H98" s="94" t="s">
+      <c r="H98" s="96" t="s">
         <v>433</v>
       </c>
       <c r="I98" s="6"/>
@@ -14764,7 +14789,7 @@
       <c r="K98" s="6"/>
     </row>
     <row r="99">
-      <c r="A99" s="86" t="s">
+      <c r="A99" s="88" t="s">
         <v>434</v>
       </c>
       <c r="B99" s="59" t="s">
@@ -14776,14 +14801,14 @@
       <c r="D99" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="E99" s="93" t="s">
+      <c r="E99" s="95" t="s">
         <v>436</v>
       </c>
       <c r="F99" s="37"/>
       <c r="G99" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H99" s="78" t="s">
+      <c r="H99" s="80" t="s">
         <v>437</v>
       </c>
       <c r="I99" s="6"/>
@@ -14797,7 +14822,7 @@
       <c r="B100" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="C100" s="95" t="s">
+      <c r="C100" s="97" t="s">
         <v>440</v>
       </c>
       <c r="D100" s="4"/>
@@ -14810,7 +14835,7 @@
       <c r="K100" s="6"/>
     </row>
     <row r="101">
-      <c r="A101" s="86" t="s">
+      <c r="A101" s="88" t="s">
         <v>441</v>
       </c>
       <c r="B101" s="59" t="s">
@@ -14837,7 +14862,7 @@
       <c r="K101" s="6"/>
     </row>
     <row r="102">
-      <c r="A102" s="86" t="s">
+      <c r="A102" s="88" t="s">
         <v>448</v>
       </c>
       <c r="B102" s="59" t="s">
@@ -14856,7 +14881,7 @@
       <c r="G102" s="37" t="s">
         <v>453</v>
       </c>
-      <c r="H102" s="78" t="s">
+      <c r="H102" s="80" t="s">
         <v>454</v>
       </c>
       <c r="I102" s="6"/>
@@ -14883,7 +14908,7 @@
       <c r="K103" s="6"/>
     </row>
     <row r="104">
-      <c r="A104" s="86" t="s">
+      <c r="A104" s="88" t="s">
         <v>457</v>
       </c>
       <c r="B104" s="59" t="s">
@@ -14929,7 +14954,7 @@
       <c r="G105" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="H105" s="78" t="s">
+      <c r="H105" s="80" t="s">
         <v>470</v>
       </c>
       <c r="I105" s="6"/>
@@ -14937,16 +14962,16 @@
       <c r="K105" s="6"/>
     </row>
     <row r="106">
-      <c r="A106" s="96" t="s">
+      <c r="A106" s="98" t="s">
         <v>464</v>
       </c>
-      <c r="B106" s="97" t="s">
+      <c r="B106" s="99" t="s">
         <v>465</v>
       </c>
-      <c r="C106" s="89" t="s">
+      <c r="C106" s="91" t="s">
         <v>466</v>
       </c>
-      <c r="D106" s="98" t="s">
+      <c r="D106" s="100" t="s">
         <v>467</v>
       </c>
       <c r="E106" s="74" t="s">
@@ -14956,7 +14981,7 @@
       <c r="G106" s="64" t="s">
         <v>469</v>
       </c>
-      <c r="H106" s="99" t="s">
+      <c r="H106" s="101" t="s">
         <v>472</v>
       </c>
       <c r="I106" s="6"/>
@@ -14964,7 +14989,7 @@
       <c r="K106" s="6"/>
     </row>
     <row r="107">
-      <c r="A107" s="92" t="s">
+      <c r="A107" s="94" t="s">
         <v>473</v>
       </c>
       <c r="B107" s="41" t="s">
@@ -15008,16 +15033,16 @@
       <c r="K108" s="6"/>
     </row>
     <row r="109">
-      <c r="A109" s="80" t="s">
+      <c r="A109" s="82" t="s">
         <v>482</v>
       </c>
-      <c r="B109" s="100"/>
-      <c r="C109" s="101"/>
-      <c r="D109" s="102"/>
-      <c r="E109" s="102" t="s">
+      <c r="B109" s="102"/>
+      <c r="C109" s="103"/>
+      <c r="D109" s="104"/>
+      <c r="E109" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="F109" s="102"/>
+      <c r="F109" s="104"/>
       <c r="G109" s="68" t="s">
         <v>483</v>
       </c>
@@ -15029,16 +15054,16 @@
       <c r="K109" s="6"/>
     </row>
     <row r="110">
-      <c r="A110" s="80" t="s">
+      <c r="A110" s="82" t="s">
         <v>485</v>
       </c>
-      <c r="B110" s="100"/>
-      <c r="C110" s="101"/>
-      <c r="D110" s="101"/>
-      <c r="E110" s="101" t="s">
+      <c r="B110" s="102"/>
+      <c r="C110" s="103"/>
+      <c r="D110" s="103"/>
+      <c r="E110" s="103" t="s">
         <v>479</v>
       </c>
-      <c r="F110" s="101"/>
+      <c r="F110" s="103"/>
       <c r="G110" s="42" t="s">
         <v>486</v>
       </c>
@@ -15067,7 +15092,7 @@
       <c r="K111" s="6"/>
     </row>
     <row r="112">
-      <c r="A112" s="86" t="s">
+      <c r="A112" s="88" t="s">
         <v>490</v>
       </c>
       <c r="B112" s="59" t="s">
@@ -15086,7 +15111,7 @@
       <c r="G112" s="64" t="s">
         <v>495</v>
       </c>
-      <c r="H112" s="99" t="s">
+      <c r="H112" s="101" t="s">
         <v>496</v>
       </c>
       <c r="I112" s="6"/>
@@ -15111,7 +15136,7 @@
       <c r="K113" s="6"/>
     </row>
     <row r="114">
-      <c r="A114" s="86" t="s">
+      <c r="A114" s="88" t="s">
         <v>499</v>
       </c>
       <c r="B114" s="59" t="s">
@@ -15138,7 +15163,7 @@
       <c r="K114" s="6"/>
     </row>
     <row r="115">
-      <c r="A115" s="103" t="s">
+      <c r="A115" s="105" t="s">
         <v>505</v>
       </c>
       <c r="B115" s="35" t="s">
@@ -15163,10 +15188,10 @@
       <c r="K115" s="6"/>
     </row>
     <row r="116">
-      <c r="A116" s="104" t="s">
+      <c r="A116" s="106" t="s">
         <v>505</v>
       </c>
-      <c r="B116" s="105" t="s">
+      <c r="B116" s="107" t="s">
         <v>506</v>
       </c>
       <c r="C116" s="64"/>
@@ -15265,7 +15290,7 @@
       <c r="G119" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="H119" s="82" t="s">
+      <c r="H119" s="84" t="s">
         <v>532</v>
       </c>
       <c r="I119" s="6"/>
@@ -15273,16 +15298,16 @@
       <c r="K119" s="6"/>
     </row>
     <row r="120">
-      <c r="A120" s="96" t="s">
+      <c r="A120" s="98" t="s">
         <v>526</v>
       </c>
-      <c r="B120" s="97" t="s">
+      <c r="B120" s="99" t="s">
         <v>527</v>
       </c>
-      <c r="C120" s="106" t="s">
+      <c r="C120" s="108" t="s">
         <v>528</v>
       </c>
-      <c r="D120" s="106" t="s">
+      <c r="D120" s="108" t="s">
         <v>529</v>
       </c>
       <c r="E120" s="51" t="s">
@@ -15292,7 +15317,7 @@
       <c r="G120" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="H120" s="82" t="s">
+      <c r="H120" s="84" t="s">
         <v>535</v>
       </c>
       <c r="I120" s="6"/>
@@ -15300,13 +15325,13 @@
       <c r="K120" s="6"/>
     </row>
     <row r="121">
-      <c r="A121" s="92" t="s">
+      <c r="A121" s="94" t="s">
         <v>536</v>
       </c>
       <c r="B121" s="41" t="s">
         <v>537</v>
       </c>
-      <c r="C121" s="107" t="s">
+      <c r="C121" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D121" s="64"/>
@@ -15325,16 +15350,16 @@
       <c r="B122" s="50" t="s">
         <v>539</v>
       </c>
-      <c r="C122" s="107" t="s">
+      <c r="C122" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D122" s="64"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="37"/>
-      <c r="G122" s="37" t="s">
+      <c r="E122" s="110"/>
+      <c r="F122" s="110"/>
+      <c r="G122" s="111" t="s">
         <v>540</v>
       </c>
-      <c r="H122" s="37" t="s">
+      <c r="H122" s="111" t="s">
         <v>541</v>
       </c>
       <c r="I122" s="6"/>
@@ -15342,7 +15367,7 @@
       <c r="K122" s="6"/>
     </row>
     <row r="123">
-      <c r="A123" s="86" t="s">
+      <c r="A123" s="88" t="s">
         <v>542</v>
       </c>
       <c r="B123" s="59" t="s">
@@ -15361,7 +15386,7 @@
       <c r="G123" s="37" t="s">
         <v>547</v>
       </c>
-      <c r="H123" s="94" t="s">
+      <c r="H123" s="96" t="s">
         <v>548</v>
       </c>
       <c r="I123" s="6"/>
@@ -15369,7 +15394,7 @@
       <c r="K123" s="6"/>
     </row>
     <row r="124">
-      <c r="A124" s="86" t="s">
+      <c r="A124" s="88" t="s">
         <v>549</v>
       </c>
       <c r="B124" s="59" t="s">
@@ -15388,7 +15413,7 @@
       <c r="G124" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="H124" s="82" t="s">
+      <c r="H124" s="84" t="s">
         <v>552</v>
       </c>
       <c r="I124" s="6"/>
@@ -15396,13 +15421,13 @@
       <c r="K124" s="6"/>
     </row>
     <row r="125">
-      <c r="A125" s="86" t="s">
+      <c r="A125" s="88" t="s">
         <v>553</v>
       </c>
       <c r="B125" s="59" t="s">
         <v>554</v>
       </c>
-      <c r="C125" s="108" t="s">
+      <c r="C125" s="112" t="s">
         <v>555</v>
       </c>
       <c r="D125" s="64"/>
@@ -15413,7 +15438,7 @@
       <c r="G125" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="H125" s="94" t="s">
+      <c r="H125" s="96" t="s">
         <v>558</v>
       </c>
       <c r="I125" s="6"/>
@@ -15421,13 +15446,13 @@
       <c r="K125" s="6"/>
     </row>
     <row r="126">
-      <c r="A126" s="92" t="s">
+      <c r="A126" s="94" t="s">
         <v>559</v>
       </c>
       <c r="B126" s="41" t="s">
         <v>506</v>
       </c>
-      <c r="C126" s="107" t="s">
+      <c r="C126" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D126" s="64"/>
@@ -15440,7 +15465,7 @@
       <c r="K126" s="6"/>
     </row>
     <row r="127">
-      <c r="A127" s="86" t="s">
+      <c r="A127" s="88" t="s">
         <v>560</v>
       </c>
       <c r="B127" s="59"/>
@@ -15461,10 +15486,10 @@
       <c r="K127" s="6"/>
     </row>
     <row r="128">
-      <c r="A128" s="86" t="s">
+      <c r="A128" s="88" t="s">
         <v>560</v>
       </c>
-      <c r="B128" s="109"/>
+      <c r="B128" s="113"/>
       <c r="C128" s="64"/>
       <c r="D128" s="6"/>
       <c r="E128" s="53" t="s">
@@ -15474,7 +15499,7 @@
       <c r="G128" s="37" t="s">
         <v>563</v>
       </c>
-      <c r="H128" s="94" t="s">
+      <c r="H128" s="96" t="s">
         <v>564</v>
       </c>
       <c r="I128" s="6"/>
@@ -15501,7 +15526,7 @@
       <c r="G129" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="H129" s="82" t="s">
+      <c r="H129" s="84" t="s">
         <v>570</v>
       </c>
       <c r="I129" s="6"/>
@@ -15515,16 +15540,16 @@
       <c r="B130" s="50" t="s">
         <v>572</v>
       </c>
-      <c r="C130" s="110"/>
-      <c r="D130" s="110"/>
-      <c r="E130" s="111" t="s">
+      <c r="C130" s="114"/>
+      <c r="D130" s="114"/>
+      <c r="E130" s="115" t="s">
         <v>530</v>
       </c>
-      <c r="F130" s="112"/>
+      <c r="F130" s="116"/>
       <c r="G130" s="53" t="s">
         <v>573</v>
       </c>
-      <c r="H130" s="113" t="s">
+      <c r="H130" s="117" t="s">
         <v>574</v>
       </c>
       <c r="I130" s="6"/>
@@ -15587,7 +15612,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="86" t="s">
+      <c r="A134" s="88" t="s">
         <v>580</v>
       </c>
       <c r="B134" s="59" t="s">
@@ -15614,7 +15639,7 @@
       <c r="K134" s="6"/>
     </row>
     <row r="135">
-      <c r="A135" s="86" t="s">
+      <c r="A135" s="88" t="s">
         <v>587</v>
       </c>
       <c r="B135" s="59" t="s">
@@ -15637,7 +15662,7 @@
       <c r="K135" s="6"/>
     </row>
     <row r="136">
-      <c r="A136" s="86" t="s">
+      <c r="A136" s="88" t="s">
         <v>592</v>
       </c>
       <c r="B136" s="59" t="s">
@@ -15660,7 +15685,7 @@
       <c r="K136" s="6"/>
     </row>
     <row r="137">
-      <c r="A137" s="86" t="s">
+      <c r="A137" s="88" t="s">
         <v>596</v>
       </c>
       <c r="B137" s="59" t="s">
@@ -15683,7 +15708,7 @@
       <c r="K137" s="6"/>
     </row>
     <row r="138">
-      <c r="A138" s="86" t="s">
+      <c r="A138" s="88" t="s">
         <v>600</v>
       </c>
       <c r="B138" s="59" t="s">
@@ -15706,13 +15731,13 @@
       <c r="K138" s="6"/>
     </row>
     <row r="139">
-      <c r="A139" s="86" t="s">
+      <c r="A139" s="88" t="s">
         <v>604</v>
       </c>
       <c r="B139" s="59" t="s">
         <v>605</v>
       </c>
-      <c r="C139" s="114" t="s">
+      <c r="C139" s="118" t="s">
         <v>606</v>
       </c>
       <c r="D139" s="64"/>
@@ -15737,7 +15762,7 @@
       <c r="B140" s="50" t="s">
         <v>609</v>
       </c>
-      <c r="C140" s="107" t="s">
+      <c r="C140" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D140" s="64"/>
@@ -15777,8 +15802,8 @@
       <c r="D142" s="73"/>
       <c r="E142" s="39"/>
       <c r="F142" s="73"/>
-      <c r="G142" s="115"/>
-      <c r="H142" s="115"/>
+      <c r="G142" s="119"/>
+      <c r="H142" s="119"/>
       <c r="I142" s="6"/>
       <c r="J142" s="6"/>
       <c r="K142" s="19" t="s">
@@ -15786,7 +15811,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="86" t="s">
+      <c r="A143" s="88" t="s">
         <v>612</v>
       </c>
       <c r="B143" s="59" t="s">
@@ -15813,7 +15838,7 @@
       <c r="K143" s="6"/>
     </row>
     <row r="144">
-      <c r="A144" s="86" t="s">
+      <c r="A144" s="88" t="s">
         <v>615</v>
       </c>
       <c r="B144" s="59" t="s">
@@ -15840,7 +15865,7 @@
       <c r="K144" s="6"/>
     </row>
     <row r="145">
-      <c r="A145" s="86" t="s">
+      <c r="A145" s="88" t="s">
         <v>618</v>
       </c>
       <c r="B145" s="59" t="s">
@@ -15867,7 +15892,7 @@
       <c r="K145" s="6"/>
     </row>
     <row r="146">
-      <c r="A146" s="86" t="s">
+      <c r="A146" s="88" t="s">
         <v>621</v>
       </c>
       <c r="B146" s="59" t="s">
@@ -15894,7 +15919,7 @@
       <c r="K146" s="6"/>
     </row>
     <row r="147">
-      <c r="A147" s="86" t="s">
+      <c r="A147" s="88" t="s">
         <v>624</v>
       </c>
       <c r="B147" s="59" t="s">
@@ -15923,7 +15948,7 @@
       <c r="K147" s="6"/>
     </row>
     <row r="148">
-      <c r="A148" s="86" t="s">
+      <c r="A148" s="88" t="s">
         <v>628</v>
       </c>
       <c r="B148" s="59" t="s">
@@ -15950,7 +15975,7 @@
       <c r="K148" s="6"/>
     </row>
     <row r="149">
-      <c r="A149" s="86" t="s">
+      <c r="A149" s="88" t="s">
         <v>632</v>
       </c>
       <c r="B149" s="59" t="s">
@@ -15977,7 +16002,7 @@
       <c r="K149" s="6"/>
     </row>
     <row r="150">
-      <c r="A150" s="86" t="s">
+      <c r="A150" s="88" t="s">
         <v>635</v>
       </c>
       <c r="B150" s="59" t="s">
@@ -15996,7 +16021,7 @@
       <c r="G150" s="53" t="s">
         <v>637</v>
       </c>
-      <c r="H150" s="94" t="s">
+      <c r="H150" s="96" t="s">
         <v>638</v>
       </c>
       <c r="I150" s="6"/>
@@ -16004,7 +16029,7 @@
       <c r="K150" s="6"/>
     </row>
     <row r="151">
-      <c r="A151" s="86" t="s">
+      <c r="A151" s="88" t="s">
         <v>639</v>
       </c>
       <c r="B151" s="59" t="s">
@@ -16023,7 +16048,7 @@
       <c r="G151" s="53" t="s">
         <v>641</v>
       </c>
-      <c r="H151" s="94" t="s">
+      <c r="H151" s="96" t="s">
         <v>642</v>
       </c>
       <c r="I151" s="6"/>
@@ -16031,7 +16056,7 @@
       <c r="K151" s="6"/>
     </row>
     <row r="152">
-      <c r="A152" s="86" t="s">
+      <c r="A152" s="88" t="s">
         <v>643</v>
       </c>
       <c r="B152" s="59" t="s">
@@ -16058,7 +16083,7 @@
       <c r="K152" s="6"/>
     </row>
     <row r="153">
-      <c r="A153" s="86" t="s">
+      <c r="A153" s="88" t="s">
         <v>647</v>
       </c>
       <c r="B153" s="59" t="s">
@@ -16085,7 +16110,7 @@
       <c r="K153" s="6"/>
     </row>
     <row r="154">
-      <c r="A154" s="86" t="s">
+      <c r="A154" s="88" t="s">
         <v>650</v>
       </c>
       <c r="B154" s="59" t="s">
@@ -16104,7 +16129,7 @@
       <c r="G154" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="H154" s="116" t="s">
+      <c r="H154" s="120" t="s">
         <v>656</v>
       </c>
       <c r="I154" s="6"/>
@@ -16112,7 +16137,7 @@
       <c r="K154" s="6"/>
     </row>
     <row r="155">
-      <c r="A155" s="76"/>
+      <c r="A155" s="79"/>
       <c r="B155" s="4"/>
       <c r="C155" s="64"/>
       <c r="D155" s="64"/>
@@ -16123,7 +16148,7 @@
       <c r="G155" s="45" t="s">
         <v>657</v>
       </c>
-      <c r="H155" s="117" t="s">
+      <c r="H155" s="121" t="s">
         <v>658</v>
       </c>
       <c r="I155" s="6"/>
@@ -16137,7 +16162,7 @@
       <c r="B156" s="50" t="s">
         <v>660</v>
       </c>
-      <c r="C156" s="107" t="s">
+      <c r="C156" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D156" s="64"/>
@@ -16186,7 +16211,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="86" t="s">
+      <c r="A159" s="88" t="s">
         <v>663</v>
       </c>
       <c r="B159" s="59" t="s">
@@ -16213,7 +16238,7 @@
       <c r="K159" s="6"/>
     </row>
     <row r="160">
-      <c r="A160" s="86" t="s">
+      <c r="A160" s="88" t="s">
         <v>669</v>
       </c>
       <c r="B160" s="59" t="s">
@@ -16240,7 +16265,7 @@
       <c r="K160" s="6"/>
     </row>
     <row r="161">
-      <c r="A161" s="86" t="s">
+      <c r="A161" s="88" t="s">
         <v>676</v>
       </c>
       <c r="B161" s="59" t="s">
@@ -16267,13 +16292,13 @@
       <c r="K161" s="6"/>
     </row>
     <row r="162">
-      <c r="A162" s="80" t="s">
+      <c r="A162" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="B162" s="81" t="s">
+      <c r="B162" s="83" t="s">
         <v>275</v>
       </c>
-      <c r="C162" s="118" t="s">
+      <c r="C162" s="122" t="s">
         <v>681</v>
       </c>
       <c r="D162" s="64"/>
@@ -16292,7 +16317,7 @@
       <c r="K162" s="6"/>
     </row>
     <row r="163">
-      <c r="A163" s="86" t="s">
+      <c r="A163" s="88" t="s">
         <v>685</v>
       </c>
       <c r="B163" s="59" t="s">
@@ -16319,13 +16344,13 @@
       <c r="K163" s="6"/>
     </row>
     <row r="164">
-      <c r="A164" s="86" t="s">
+      <c r="A164" s="88" t="s">
         <v>688</v>
       </c>
       <c r="B164" s="59" t="s">
         <v>275</v>
       </c>
-      <c r="C164" s="118" t="s">
+      <c r="C164" s="122" t="s">
         <v>681</v>
       </c>
       <c r="D164" s="64"/>
@@ -16350,7 +16375,7 @@
       <c r="B165" s="50" t="s">
         <v>691</v>
       </c>
-      <c r="C165" s="107" t="s">
+      <c r="C165" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D165" s="64"/>
@@ -16363,7 +16388,7 @@
       <c r="K165" s="6"/>
     </row>
     <row r="166">
-      <c r="A166" s="86" t="s">
+      <c r="A166" s="88" t="s">
         <v>692</v>
       </c>
       <c r="B166" s="59" t="s">
@@ -16382,7 +16407,7 @@
       <c r="G166" s="53" t="s">
         <v>697</v>
       </c>
-      <c r="H166" s="119" t="s">
+      <c r="H166" s="123" t="s">
         <v>698</v>
       </c>
       <c r="I166" s="6"/>
@@ -16390,7 +16415,7 @@
       <c r="K166" s="6"/>
     </row>
     <row r="167">
-      <c r="A167" s="86" t="s">
+      <c r="A167" s="88" t="s">
         <v>699</v>
       </c>
       <c r="B167" s="59" t="s">
@@ -16407,7 +16432,7 @@
       <c r="K167" s="6"/>
     </row>
     <row r="168">
-      <c r="A168" s="86" t="s">
+      <c r="A168" s="88" t="s">
         <v>701</v>
       </c>
       <c r="B168" s="59" t="s">
@@ -16419,10 +16444,10 @@
       <c r="D168" s="74" t="s">
         <v>704</v>
       </c>
-      <c r="E168" s="120" t="s">
+      <c r="E168" s="124" t="s">
         <v>705</v>
       </c>
-      <c r="F168" s="120"/>
+      <c r="F168" s="124"/>
       <c r="G168" s="37" t="s">
         <v>706</v>
       </c>
@@ -16434,20 +16459,20 @@
       <c r="K168" s="6"/>
     </row>
     <row r="169">
-      <c r="A169" s="86" t="s">
+      <c r="A169" s="88" t="s">
         <v>708</v>
       </c>
       <c r="B169" s="59" t="s">
         <v>275</v>
       </c>
-      <c r="C169" s="118" t="s">
+      <c r="C169" s="122" t="s">
         <v>681</v>
       </c>
       <c r="D169" s="64"/>
-      <c r="E169" s="120" t="s">
+      <c r="E169" s="124" t="s">
         <v>709</v>
       </c>
-      <c r="F169" s="120"/>
+      <c r="F169" s="124"/>
       <c r="G169" s="53" t="s">
         <v>710</v>
       </c>
@@ -16459,7 +16484,7 @@
       <c r="K169" s="6"/>
     </row>
     <row r="170">
-      <c r="A170" s="86" t="s">
+      <c r="A170" s="88" t="s">
         <v>712</v>
       </c>
       <c r="B170" s="59" t="s">
@@ -16471,10 +16496,10 @@
       <c r="D170" s="64" t="s">
         <v>715</v>
       </c>
-      <c r="E170" s="120" t="s">
+      <c r="E170" s="124" t="s">
         <v>716</v>
       </c>
-      <c r="F170" s="120"/>
+      <c r="F170" s="124"/>
       <c r="G170" s="74" t="s">
         <v>717</v>
       </c>
@@ -16486,7 +16511,7 @@
       <c r="K170" s="6"/>
     </row>
     <row r="171">
-      <c r="A171" s="86" t="s">
+      <c r="A171" s="88" t="s">
         <v>719</v>
       </c>
       <c r="B171" s="59" t="s">
@@ -16498,10 +16523,10 @@
       <c r="D171" s="37" t="s">
         <v>722</v>
       </c>
-      <c r="E171" s="120" t="s">
+      <c r="E171" s="124" t="s">
         <v>723</v>
       </c>
-      <c r="F171" s="120"/>
+      <c r="F171" s="124"/>
       <c r="G171" s="53" t="s">
         <v>724</v>
       </c>
@@ -16516,13 +16541,13 @@
       <c r="A172" s="71" t="s">
         <v>726</v>
       </c>
-      <c r="B172" s="121" t="s">
+      <c r="B172" s="125" t="s">
         <v>727</v>
       </c>
       <c r="C172" s="73"/>
       <c r="D172" s="73"/>
-      <c r="E172" s="122"/>
-      <c r="F172" s="123"/>
+      <c r="E172" s="126"/>
+      <c r="F172" s="127"/>
       <c r="G172" s="73"/>
       <c r="H172" s="73"/>
       <c r="I172" s="6"/>
@@ -16537,11 +16562,11 @@
         <v>702</v>
       </c>
       <c r="C173" s="73"/>
-      <c r="D173" s="124"/>
-      <c r="E173" s="125" t="s">
+      <c r="D173" s="128"/>
+      <c r="E173" s="129" t="s">
         <v>729</v>
       </c>
-      <c r="F173" s="123"/>
+      <c r="F173" s="127"/>
       <c r="G173" s="65" t="s">
         <v>730</v>
       </c>
@@ -16560,11 +16585,11 @@
         <v>275</v>
       </c>
       <c r="C174" s="73"/>
-      <c r="D174" s="124"/>
-      <c r="E174" s="125" t="s">
+      <c r="D174" s="128"/>
+      <c r="E174" s="129" t="s">
         <v>733</v>
       </c>
-      <c r="F174" s="123"/>
+      <c r="F174" s="127"/>
       <c r="G174" s="65" t="s">
         <v>734</v>
       </c>
@@ -16579,12 +16604,12 @@
       <c r="A175" s="71" t="s">
         <v>736</v>
       </c>
-      <c r="B175" s="121" t="s">
+      <c r="B175" s="125" t="s">
         <v>737</v>
       </c>
       <c r="C175" s="73"/>
-      <c r="D175" s="124"/>
-      <c r="E175" s="126" t="s">
+      <c r="D175" s="128"/>
+      <c r="E175" s="130" t="s">
         <v>738</v>
       </c>
       <c r="F175" s="39"/>
@@ -16659,7 +16684,7 @@
       <c r="G179" s="65" t="s">
         <v>746</v>
       </c>
-      <c r="H179" s="127" t="s">
+      <c r="H179" s="131" t="s">
         <v>747</v>
       </c>
       <c r="I179" s="6"/>
@@ -16692,10 +16717,10 @@
       <c r="B181" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="C181" s="128" t="s">
+      <c r="C181" s="132" t="s">
         <v>752</v>
       </c>
-      <c r="D181" s="129" t="s">
+      <c r="D181" s="133" t="s">
         <v>753</v>
       </c>
       <c r="E181" s="65" t="s">
@@ -16719,8 +16744,8 @@
       <c r="B182" s="72"/>
       <c r="C182" s="73"/>
       <c r="D182" s="73"/>
-      <c r="E182" s="130"/>
-      <c r="F182" s="123"/>
+      <c r="E182" s="134"/>
+      <c r="F182" s="127"/>
       <c r="G182" s="65"/>
       <c r="H182" s="65"/>
       <c r="I182" s="6"/>
@@ -16734,8 +16759,8 @@
       <c r="B183" s="72"/>
       <c r="C183" s="73"/>
       <c r="D183" s="73"/>
-      <c r="E183" s="130"/>
-      <c r="F183" s="123"/>
+      <c r="E183" s="134"/>
+      <c r="F183" s="127"/>
       <c r="G183" s="65"/>
       <c r="H183" s="65"/>
       <c r="I183" s="6"/>
@@ -16751,16 +16776,16 @@
       <c r="B184" s="70" t="s">
         <v>757</v>
       </c>
-      <c r="C184" s="128" t="s">
+      <c r="C184" s="132" t="s">
         <v>758</v>
       </c>
-      <c r="D184" s="129" t="s">
+      <c r="D184" s="133" t="s">
         <v>759</v>
       </c>
-      <c r="E184" s="130" t="s">
+      <c r="E184" s="134" t="s">
         <v>760</v>
       </c>
-      <c r="F184" s="123"/>
+      <c r="F184" s="127"/>
       <c r="G184" s="39" t="s">
         <v>761</v>
       </c>
@@ -16778,10 +16803,10 @@
       <c r="B185" s="70" t="s">
         <v>764</v>
       </c>
-      <c r="C185" s="131" t="s">
+      <c r="C185" s="135" t="s">
         <v>765</v>
       </c>
-      <c r="D185" s="132" t="s">
+      <c r="D185" s="136" t="s">
         <v>766</v>
       </c>
       <c r="E185" s="65" t="s">
@@ -16795,7 +16820,7 @@
       <c r="K185" s="6"/>
     </row>
     <row r="186">
-      <c r="A186" s="103" t="s">
+      <c r="A186" s="105" t="s">
         <v>768</v>
       </c>
       <c r="B186" s="35" t="s">
@@ -16812,7 +16837,7 @@
       <c r="K186" s="6"/>
     </row>
     <row r="187">
-      <c r="A187" s="92" t="s">
+      <c r="A187" s="94" t="s">
         <v>770</v>
       </c>
       <c r="B187" s="41" t="s">
@@ -16824,14 +16849,14 @@
       <c r="D187" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="E187" s="120" t="s">
+      <c r="E187" s="124" t="s">
         <v>771</v>
       </c>
-      <c r="F187" s="120"/>
-      <c r="G187" s="133" t="s">
+      <c r="F187" s="124"/>
+      <c r="G187" s="137" t="s">
         <v>209</v>
       </c>
-      <c r="H187" s="134" t="s">
+      <c r="H187" s="138" t="s">
         <v>772</v>
       </c>
       <c r="I187" s="6"/>
@@ -16839,18 +16864,18 @@
       <c r="K187" s="6"/>
     </row>
     <row r="188">
-      <c r="A188" s="92" t="s">
+      <c r="A188" s="94" t="s">
         <v>773</v>
       </c>
       <c r="B188" s="41" t="s">
         <v>774</v>
       </c>
-      <c r="C188" s="107" t="s">
+      <c r="C188" s="109" t="s">
         <v>440</v>
       </c>
       <c r="D188" s="6"/>
-      <c r="E188" s="135"/>
-      <c r="F188" s="135"/>
+      <c r="E188" s="139"/>
+      <c r="F188" s="139"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
       <c r="I188" s="6"/>
@@ -16864,7 +16889,7 @@
       <c r="B189" s="50" t="s">
         <v>776</v>
       </c>
-      <c r="C189" s="136" t="s">
+      <c r="C189" s="140" t="s">
         <v>440</v>
       </c>
       <c r="D189" s="6"/>
@@ -16883,7 +16908,7 @@
       <c r="K189" s="6"/>
     </row>
     <row r="190">
-      <c r="A190" s="86" t="s">
+      <c r="A190" s="88" t="s">
         <v>780</v>
       </c>
       <c r="B190" s="59" t="s">
@@ -16910,7 +16935,7 @@
       <c r="K190" s="6"/>
     </row>
     <row r="191">
-      <c r="A191" s="86" t="s">
+      <c r="A191" s="88" t="s">
         <v>783</v>
       </c>
       <c r="B191" s="59" t="s">
@@ -16937,7 +16962,7 @@
       <c r="K191" s="6"/>
     </row>
     <row r="192">
-      <c r="A192" s="86" t="s">
+      <c r="A192" s="88" t="s">
         <v>786</v>
       </c>
       <c r="B192" s="59" t="s">
@@ -16964,7 +16989,7 @@
       <c r="K192" s="6"/>
     </row>
     <row r="193">
-      <c r="A193" s="86" t="s">
+      <c r="A193" s="88" t="s">
         <v>789</v>
       </c>
       <c r="B193" s="59" t="s">
@@ -16991,7 +17016,7 @@
       <c r="K193" s="6"/>
     </row>
     <row r="194">
-      <c r="A194" s="86" t="s">
+      <c r="A194" s="88" t="s">
         <v>793</v>
       </c>
       <c r="B194" s="59" t="s">
@@ -17018,7 +17043,7 @@
       <c r="K194" s="6"/>
     </row>
     <row r="195">
-      <c r="A195" s="86" t="s">
+      <c r="A195" s="88" t="s">
         <v>796</v>
       </c>
       <c r="B195" s="59" t="s">
@@ -17045,7 +17070,7 @@
       <c r="K195" s="6"/>
     </row>
     <row r="196">
-      <c r="A196" s="86" t="s">
+      <c r="A196" s="88" t="s">
         <v>798</v>
       </c>
       <c r="B196" s="59" t="s">
@@ -17072,7 +17097,7 @@
       <c r="K196" s="6"/>
     </row>
     <row r="197">
-      <c r="A197" s="86" t="s">
+      <c r="A197" s="88" t="s">
         <v>800</v>
       </c>
       <c r="B197" s="59" t="s">
@@ -17099,7 +17124,7 @@
       <c r="K197" s="6"/>
     </row>
     <row r="198">
-      <c r="A198" s="86" t="s">
+      <c r="A198" s="88" t="s">
         <v>803</v>
       </c>
       <c r="B198" s="59" t="s">
@@ -17132,10 +17157,10 @@
       <c r="B199" s="50" t="s">
         <v>806</v>
       </c>
-      <c r="C199" s="137" t="s">
+      <c r="C199" s="141" t="s">
         <v>440</v>
       </c>
-      <c r="D199" s="138"/>
+      <c r="D199" s="142"/>
       <c r="E199" s="4" t="s">
         <v>777</v>
       </c>
@@ -17151,7 +17176,7 @@
       <c r="K199" s="6"/>
     </row>
     <row r="200">
-      <c r="A200" s="86" t="s">
+      <c r="A200" s="88" t="s">
         <v>808</v>
       </c>
       <c r="B200" s="59" t="s">
@@ -17178,7 +17203,7 @@
       <c r="K200" s="6"/>
     </row>
     <row r="201">
-      <c r="A201" s="86" t="s">
+      <c r="A201" s="88" t="s">
         <v>811</v>
       </c>
       <c r="B201" s="59" t="s">
@@ -17205,7 +17230,7 @@
       <c r="K201" s="6"/>
     </row>
     <row r="202">
-      <c r="A202" s="86" t="s">
+      <c r="A202" s="88" t="s">
         <v>814</v>
       </c>
       <c r="B202" s="59" t="s">
@@ -17232,7 +17257,7 @@
       <c r="K202" s="6"/>
     </row>
     <row r="203">
-      <c r="A203" s="86" t="s">
+      <c r="A203" s="88" t="s">
         <v>817</v>
       </c>
       <c r="B203" s="59" t="s">
@@ -17259,16 +17284,16 @@
       <c r="K203" s="6"/>
     </row>
     <row r="204">
-      <c r="A204" s="86" t="s">
+      <c r="A204" s="88" t="s">
         <v>820</v>
       </c>
       <c r="B204" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C204" s="139" t="s">
+      <c r="C204" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="D204" s="139" t="s">
+      <c r="D204" s="143" t="s">
         <v>99</v>
       </c>
       <c r="E204" s="53" t="s">
@@ -17286,7 +17311,7 @@
       <c r="K204" s="6"/>
     </row>
     <row r="205">
-      <c r="A205" s="86" t="s">
+      <c r="A205" s="88" t="s">
         <v>823</v>
       </c>
       <c r="B205" s="59" t="s">
@@ -17313,7 +17338,7 @@
       <c r="K205" s="6"/>
     </row>
     <row r="206">
-      <c r="A206" s="86" t="s">
+      <c r="A206" s="88" t="s">
         <v>825</v>
       </c>
       <c r="B206" s="59" t="s">
@@ -17340,7 +17365,7 @@
       <c r="K206" s="6"/>
     </row>
     <row r="207">
-      <c r="A207" s="86" t="s">
+      <c r="A207" s="88" t="s">
         <v>827</v>
       </c>
       <c r="B207" s="59" t="s">
@@ -17367,7 +17392,7 @@
       <c r="K207" s="6"/>
     </row>
     <row r="208">
-      <c r="A208" s="86" t="s">
+      <c r="A208" s="88" t="s">
         <v>830</v>
       </c>
       <c r="B208" s="59" t="s">
@@ -17410,10 +17435,10 @@
         <v>836</v>
       </c>
       <c r="F209" s="64"/>
-      <c r="G209" s="133" t="s">
+      <c r="G209" s="137" t="s">
         <v>837</v>
       </c>
-      <c r="H209" s="140" t="s">
+      <c r="H209" s="144" t="s">
         <v>838</v>
       </c>
       <c r="I209" s="6"/>
@@ -17436,7 +17461,7 @@
       <c r="G210" s="37" t="s">
         <v>841</v>
       </c>
-      <c r="H210" s="113" t="s">
+      <c r="H210" s="117" t="s">
         <v>779</v>
       </c>
       <c r="I210" s="6"/>
@@ -17444,7 +17469,7 @@
       <c r="K210" s="6"/>
     </row>
     <row r="211">
-      <c r="A211" s="86" t="s">
+      <c r="A211" s="88" t="s">
         <v>842</v>
       </c>
       <c r="B211" s="59" t="s">
@@ -17460,10 +17485,10 @@
         <v>843</v>
       </c>
       <c r="F211" s="74"/>
-      <c r="G211" s="77" t="s">
+      <c r="G211" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="H211" s="141" t="s">
+      <c r="H211" s="145" t="s">
         <v>844</v>
       </c>
       <c r="I211" s="6"/>
@@ -17471,7 +17496,7 @@
       <c r="K211" s="6"/>
     </row>
     <row r="212">
-      <c r="A212" s="86" t="s">
+      <c r="A212" s="88" t="s">
         <v>845</v>
       </c>
       <c r="B212" s="59" t="s">
@@ -17490,7 +17515,7 @@
       <c r="G212" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="H212" s="82" t="s">
+      <c r="H212" s="84" t="s">
         <v>847</v>
       </c>
       <c r="I212" s="6"/>
@@ -17498,7 +17523,7 @@
       <c r="K212" s="6"/>
     </row>
     <row r="213">
-      <c r="A213" s="86" t="s">
+      <c r="A213" s="88" t="s">
         <v>848</v>
       </c>
       <c r="B213" s="59" t="s">
@@ -17517,7 +17542,7 @@
       <c r="G213" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="H213" s="82" t="s">
+      <c r="H213" s="84" t="s">
         <v>850</v>
       </c>
       <c r="I213" s="6"/>
@@ -17525,7 +17550,7 @@
       <c r="K213" s="6"/>
     </row>
     <row r="214">
-      <c r="A214" s="86" t="s">
+      <c r="A214" s="88" t="s">
         <v>851</v>
       </c>
       <c r="B214" s="59" t="s">
@@ -17552,7 +17577,7 @@
       <c r="K214" s="6"/>
     </row>
     <row r="215">
-      <c r="A215" s="86" t="s">
+      <c r="A215" s="88" t="s">
         <v>854</v>
       </c>
       <c r="B215" s="59" t="s">
@@ -17571,7 +17596,7 @@
       <c r="G215" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="H215" s="94" t="s">
+      <c r="H215" s="96" t="s">
         <v>856</v>
       </c>
       <c r="I215" s="6"/>
@@ -17579,7 +17604,7 @@
       <c r="K215" s="6"/>
     </row>
     <row r="216">
-      <c r="A216" s="86" t="s">
+      <c r="A216" s="88" t="s">
         <v>857</v>
       </c>
       <c r="B216" s="59" t="s">
@@ -17606,7 +17631,7 @@
       <c r="K216" s="6"/>
     </row>
     <row r="217">
-      <c r="A217" s="86" t="s">
+      <c r="A217" s="88" t="s">
         <v>859</v>
       </c>
       <c r="B217" s="59" t="s">
@@ -17633,7 +17658,7 @@
       <c r="K217" s="6"/>
     </row>
     <row r="218">
-      <c r="A218" s="86" t="s">
+      <c r="A218" s="88" t="s">
         <v>861</v>
       </c>
       <c r="B218" s="59" t="s">
@@ -17660,7 +17685,7 @@
       <c r="K218" s="6"/>
     </row>
     <row r="219">
-      <c r="A219" s="86" t="s">
+      <c r="A219" s="88" t="s">
         <v>864</v>
       </c>
       <c r="B219" s="59" t="s">
@@ -17679,7 +17704,7 @@
       <c r="G219" s="53" t="s">
         <v>641</v>
       </c>
-      <c r="H219" s="94" t="s">
+      <c r="H219" s="96" t="s">
         <v>649</v>
       </c>
       <c r="I219" s="6"/>
@@ -17687,26 +17712,26 @@
       <c r="K219" s="6"/>
     </row>
     <row r="220">
-      <c r="A220" s="92" t="s">
+      <c r="A220" s="94" t="s">
         <v>866</v>
       </c>
       <c r="B220" s="41" t="s">
         <v>867</v>
       </c>
-      <c r="C220" s="142" t="s">
+      <c r="C220" s="146" t="s">
         <v>868</v>
       </c>
-      <c r="D220" s="142" t="s">
+      <c r="D220" s="146" t="s">
         <v>869</v>
       </c>
-      <c r="E220" s="143" t="s">
+      <c r="E220" s="147" t="s">
         <v>870</v>
       </c>
-      <c r="F220" s="143"/>
-      <c r="G220" s="144" t="s">
+      <c r="F220" s="147"/>
+      <c r="G220" s="148" t="s">
         <v>871</v>
       </c>
-      <c r="H220" s="145" t="s">
+      <c r="H220" s="149" t="s">
         <v>872</v>
       </c>
       <c r="I220" s="6"/>
@@ -17717,7 +17742,7 @@
       <c r="A221" s="69" t="s">
         <v>873</v>
       </c>
-      <c r="B221" s="146" t="s">
+      <c r="B221" s="150" t="s">
         <v>874</v>
       </c>
       <c r="C221" s="73"/>
@@ -17734,14 +17759,14 @@
       <c r="A222" s="69" t="s">
         <v>875</v>
       </c>
-      <c r="B222" s="146" t="s">
+      <c r="B222" s="150" t="s">
         <v>876</v>
       </c>
-      <c r="C222" s="147" t="s">
+      <c r="C222" s="151" t="s">
         <v>440</v>
       </c>
       <c r="D222" s="73"/>
-      <c r="E222" s="148" t="s">
+      <c r="E222" s="152" t="s">
         <v>877</v>
       </c>
       <c r="F222" s="73"/>
@@ -17755,7 +17780,7 @@
       <c r="A223" s="69" t="s">
         <v>878</v>
       </c>
-      <c r="B223" s="146" t="s">
+      <c r="B223" s="150" t="s">
         <v>879</v>
       </c>
       <c r="C223" s="73" t="s">
@@ -17764,14 +17789,14 @@
       <c r="D223" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E223" s="149" t="s">
+      <c r="E223" s="153" t="s">
         <v>882</v>
       </c>
       <c r="F223" s="73"/>
-      <c r="G223" s="149" t="s">
+      <c r="G223" s="153" t="s">
         <v>883</v>
       </c>
-      <c r="H223" s="150" t="s">
+      <c r="H223" s="154" t="s">
         <v>884</v>
       </c>
       <c r="I223" s="6"/>
@@ -17782,7 +17807,7 @@
       <c r="A224" s="69" t="s">
         <v>885</v>
       </c>
-      <c r="B224" s="146" t="s">
+      <c r="B224" s="150" t="s">
         <v>886</v>
       </c>
       <c r="C224" s="73" t="s">
@@ -17798,7 +17823,7 @@
       <c r="G224" s="65" t="s">
         <v>883</v>
       </c>
-      <c r="H224" s="127" t="s">
+      <c r="H224" s="131" t="s">
         <v>888</v>
       </c>
       <c r="I224" s="6"/>
@@ -17809,7 +17834,7 @@
       <c r="A225" s="69" t="s">
         <v>889</v>
       </c>
-      <c r="B225" s="146" t="s">
+      <c r="B225" s="150" t="s">
         <v>890</v>
       </c>
       <c r="C225" s="73"/>
@@ -17826,7 +17851,7 @@
       <c r="A226" s="69" t="s">
         <v>891</v>
       </c>
-      <c r="B226" s="146" t="s">
+      <c r="B226" s="150" t="s">
         <v>892</v>
       </c>
       <c r="C226" s="73" t="s">
@@ -17835,14 +17860,14 @@
       <c r="D226" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E226" s="151" t="s">
+      <c r="E226" s="155" t="s">
         <v>893</v>
       </c>
       <c r="F226" s="73"/>
       <c r="G226" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H226" s="150" t="s">
+      <c r="H226" s="154" t="s">
         <v>894</v>
       </c>
       <c r="I226" s="6"/>
@@ -17853,7 +17878,7 @@
       <c r="A227" s="69" t="s">
         <v>895</v>
       </c>
-      <c r="B227" s="146" t="s">
+      <c r="B227" s="150" t="s">
         <v>896</v>
       </c>
       <c r="C227" s="73" t="s">
@@ -17862,14 +17887,14 @@
       <c r="D227" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E227" s="151" t="s">
+      <c r="E227" s="155" t="s">
         <v>897</v>
       </c>
       <c r="F227" s="73"/>
       <c r="G227" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H227" s="150" t="s">
+      <c r="H227" s="154" t="s">
         <v>898</v>
       </c>
       <c r="I227" s="6"/>
@@ -17880,7 +17905,7 @@
       <c r="A228" s="69" t="s">
         <v>899</v>
       </c>
-      <c r="B228" s="146" t="s">
+      <c r="B228" s="150" t="s">
         <v>900</v>
       </c>
       <c r="C228" s="73" t="s">
@@ -17889,14 +17914,14 @@
       <c r="D228" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E228" s="151" t="s">
+      <c r="E228" s="155" t="s">
         <v>901</v>
       </c>
       <c r="F228" s="73"/>
       <c r="G228" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H228" s="150" t="s">
+      <c r="H228" s="154" t="s">
         <v>902</v>
       </c>
       <c r="I228" s="6"/>
@@ -17907,23 +17932,23 @@
       <c r="A229" s="69" t="s">
         <v>903</v>
       </c>
-      <c r="B229" s="146" t="s">
+      <c r="B229" s="150" t="s">
         <v>904</v>
       </c>
-      <c r="C229" s="152" t="s">
+      <c r="C229" s="156" t="s">
         <v>880</v>
       </c>
       <c r="D229" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E229" s="151" t="s">
+      <c r="E229" s="155" t="s">
         <v>905</v>
       </c>
       <c r="F229" s="73"/>
       <c r="G229" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H229" s="150" t="s">
+      <c r="H229" s="154" t="s">
         <v>906</v>
       </c>
       <c r="I229" s="6"/>
@@ -17934,23 +17959,23 @@
       <c r="A230" s="69" t="s">
         <v>907</v>
       </c>
-      <c r="B230" s="146" t="s">
+      <c r="B230" s="150" t="s">
         <v>908</v>
       </c>
-      <c r="C230" s="152" t="s">
+      <c r="C230" s="156" t="s">
         <v>880</v>
       </c>
       <c r="D230" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E230" s="151" t="s">
+      <c r="E230" s="155" t="s">
         <v>909</v>
       </c>
       <c r="F230" s="73"/>
       <c r="G230" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H230" s="150" t="s">
+      <c r="H230" s="154" t="s">
         <v>910</v>
       </c>
       <c r="I230" s="6"/>
@@ -17961,23 +17986,23 @@
       <c r="A231" s="69" t="s">
         <v>911</v>
       </c>
-      <c r="B231" s="146" t="s">
+      <c r="B231" s="150" t="s">
         <v>912</v>
       </c>
-      <c r="C231" s="152" t="s">
+      <c r="C231" s="156" t="s">
         <v>880</v>
       </c>
       <c r="D231" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E231" s="151" t="s">
+      <c r="E231" s="155" t="s">
         <v>913</v>
       </c>
       <c r="F231" s="73"/>
       <c r="G231" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H231" s="150" t="s">
+      <c r="H231" s="154" t="s">
         <v>914</v>
       </c>
       <c r="I231" s="6"/>
@@ -17988,23 +18013,23 @@
       <c r="A232" s="69" t="s">
         <v>915</v>
       </c>
-      <c r="B232" s="146" t="s">
+      <c r="B232" s="150" t="s">
         <v>916</v>
       </c>
-      <c r="C232" s="152" t="s">
+      <c r="C232" s="156" t="s">
         <v>880</v>
       </c>
       <c r="D232" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E232" s="151" t="s">
+      <c r="E232" s="155" t="s">
         <v>917</v>
       </c>
       <c r="F232" s="73"/>
       <c r="G232" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H232" s="150" t="s">
+      <c r="H232" s="154" t="s">
         <v>918</v>
       </c>
       <c r="I232" s="6"/>
@@ -18015,23 +18040,23 @@
       <c r="A233" s="69" t="s">
         <v>919</v>
       </c>
-      <c r="B233" s="146" t="s">
+      <c r="B233" s="150" t="s">
         <v>920</v>
       </c>
-      <c r="C233" s="147" t="s">
+      <c r="C233" s="151" t="s">
         <v>880</v>
       </c>
-      <c r="D233" s="149" t="s">
+      <c r="D233" s="153" t="s">
         <v>881</v>
       </c>
-      <c r="E233" s="149" t="s">
+      <c r="E233" s="153" t="s">
         <v>921</v>
       </c>
       <c r="F233" s="73"/>
       <c r="G233" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H233" s="150" t="s">
+      <c r="H233" s="154" t="s">
         <v>922</v>
       </c>
       <c r="I233" s="6"/>
@@ -18042,14 +18067,14 @@
       <c r="A234" s="69" t="s">
         <v>923</v>
       </c>
-      <c r="B234" s="146" t="s">
+      <c r="B234" s="150" t="s">
         <v>924</v>
       </c>
-      <c r="C234" s="147" t="s">
+      <c r="C234" s="151" t="s">
         <v>440</v>
       </c>
-      <c r="D234" s="149"/>
-      <c r="E234" s="149"/>
+      <c r="D234" s="153"/>
+      <c r="E234" s="153"/>
       <c r="F234" s="73"/>
       <c r="G234" s="73"/>
       <c r="H234" s="73"/>
@@ -18061,23 +18086,23 @@
       <c r="A235" s="69" t="s">
         <v>925</v>
       </c>
-      <c r="B235" s="146" t="s">
+      <c r="B235" s="150" t="s">
         <v>926</v>
       </c>
-      <c r="C235" s="149" t="s">
+      <c r="C235" s="153" t="s">
         <v>880</v>
       </c>
-      <c r="D235" s="149" t="s">
+      <c r="D235" s="153" t="s">
         <v>881</v>
       </c>
-      <c r="E235" s="149" t="s">
+      <c r="E235" s="153" t="s">
         <v>927</v>
       </c>
       <c r="F235" s="73"/>
       <c r="G235" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H235" s="150" t="s">
+      <c r="H235" s="154" t="s">
         <v>928</v>
       </c>
       <c r="I235" s="6"/>
@@ -18088,23 +18113,23 @@
       <c r="A236" s="69" t="s">
         <v>929</v>
       </c>
-      <c r="B236" s="146" t="s">
+      <c r="B236" s="150" t="s">
         <v>930</v>
       </c>
-      <c r="C236" s="149" t="s">
+      <c r="C236" s="153" t="s">
         <v>880</v>
       </c>
-      <c r="D236" s="149" t="s">
+      <c r="D236" s="153" t="s">
         <v>881</v>
       </c>
-      <c r="E236" s="149" t="s">
+      <c r="E236" s="153" t="s">
         <v>931</v>
       </c>
       <c r="F236" s="73"/>
       <c r="G236" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H236" s="150" t="s">
+      <c r="H236" s="154" t="s">
         <v>932</v>
       </c>
       <c r="I236" s="6"/>
@@ -18115,7 +18140,7 @@
       <c r="A237" s="69" t="s">
         <v>933</v>
       </c>
-      <c r="B237" s="146" t="s">
+      <c r="B237" s="150" t="s">
         <v>934</v>
       </c>
       <c r="C237" s="73" t="s">
@@ -18124,14 +18149,14 @@
       <c r="D237" s="73" t="s">
         <v>881</v>
       </c>
-      <c r="E237" s="151" t="s">
+      <c r="E237" s="155" t="s">
         <v>935</v>
       </c>
       <c r="F237" s="73"/>
-      <c r="G237" s="149" t="s">
+      <c r="G237" s="153" t="s">
         <v>883</v>
       </c>
-      <c r="H237" s="150" t="s">
+      <c r="H237" s="154" t="s">
         <v>936</v>
       </c>
       <c r="I237" s="6"/>
@@ -18142,12 +18167,12 @@
       <c r="A238" s="69" t="s">
         <v>937</v>
       </c>
-      <c r="B238" s="146" t="s">
+      <c r="B238" s="150" t="s">
         <v>938</v>
       </c>
-      <c r="C238" s="149"/>
-      <c r="D238" s="149"/>
-      <c r="E238" s="149"/>
+      <c r="C238" s="153"/>
+      <c r="D238" s="153"/>
+      <c r="E238" s="153"/>
       <c r="F238" s="73"/>
       <c r="G238" s="73"/>
       <c r="H238" s="73"/>
@@ -18159,21 +18184,21 @@
       <c r="A239" s="69" t="s">
         <v>939</v>
       </c>
-      <c r="B239" s="146" t="s">
+      <c r="B239" s="150" t="s">
         <v>940</v>
       </c>
-      <c r="C239" s="153" t="s">
+      <c r="C239" s="157" t="s">
         <v>555</v>
       </c>
       <c r="D239" s="73"/>
-      <c r="E239" s="149" t="s">
+      <c r="E239" s="153" t="s">
         <v>941</v>
       </c>
       <c r="F239" s="73"/>
       <c r="G239" s="73" t="s">
         <v>883</v>
       </c>
-      <c r="H239" s="150" t="s">
+      <c r="H239" s="154" t="s">
         <v>942</v>
       </c>
       <c r="I239" s="6"/>
@@ -18184,12 +18209,12 @@
       <c r="A240" s="69" t="s">
         <v>943</v>
       </c>
-      <c r="B240" s="146" t="s">
+      <c r="B240" s="150" t="s">
         <v>944</v>
       </c>
-      <c r="C240" s="149"/>
-      <c r="D240" s="149"/>
-      <c r="E240" s="149"/>
+      <c r="C240" s="153"/>
+      <c r="D240" s="153"/>
+      <c r="E240" s="153"/>
       <c r="F240" s="73"/>
       <c r="G240" s="73"/>
       <c r="H240" s="73"/>
@@ -18201,23 +18226,23 @@
       <c r="A241" s="69" t="s">
         <v>945</v>
       </c>
-      <c r="B241" s="146" t="s">
+      <c r="B241" s="150" t="s">
         <v>946</v>
       </c>
-      <c r="C241" s="147" t="s">
+      <c r="C241" s="151" t="s">
         <v>947</v>
       </c>
-      <c r="D241" s="149" t="s">
+      <c r="D241" s="153" t="s">
         <v>948</v>
       </c>
-      <c r="E241" s="154" t="s">
+      <c r="E241" s="158" t="s">
         <v>949</v>
       </c>
       <c r="F241" s="73"/>
       <c r="G241" s="73" t="s">
         <v>950</v>
       </c>
-      <c r="H241" s="149" t="s">
+      <c r="H241" s="153" t="s">
         <v>951</v>
       </c>
       <c r="I241" s="6"/>
@@ -18225,322 +18250,322 @@
       <c r="K241" s="6"/>
     </row>
     <row r="242">
-      <c r="A242" s="155"/>
+      <c r="A242" s="159"/>
       <c r="G242" s="29"/>
       <c r="H242" s="29"/>
     </row>
     <row r="243">
-      <c r="A243" s="155"/>
+      <c r="A243" s="159"/>
       <c r="G243" s="29"/>
       <c r="H243" s="29"/>
     </row>
     <row r="244">
-      <c r="A244" s="155"/>
+      <c r="A244" s="159"/>
       <c r="G244" s="29"/>
       <c r="H244" s="29"/>
     </row>
     <row r="245">
-      <c r="A245" s="155"/>
+      <c r="A245" s="159"/>
       <c r="G245" s="29"/>
       <c r="H245" s="29"/>
     </row>
     <row r="246">
-      <c r="A246" s="155"/>
+      <c r="A246" s="159"/>
       <c r="G246" s="29"/>
       <c r="H246" s="29"/>
     </row>
     <row r="247">
-      <c r="A247" s="155"/>
+      <c r="A247" s="159"/>
       <c r="G247" s="29"/>
       <c r="H247" s="29"/>
     </row>
     <row r="248">
-      <c r="A248" s="155"/>
+      <c r="A248" s="159"/>
       <c r="G248" s="29"/>
       <c r="H248" s="29"/>
     </row>
     <row r="249">
-      <c r="A249" s="155"/>
+      <c r="A249" s="159"/>
       <c r="G249" s="29"/>
       <c r="H249" s="29"/>
     </row>
     <row r="250">
-      <c r="A250" s="155"/>
+      <c r="A250" s="159"/>
       <c r="G250" s="29"/>
       <c r="H250" s="29"/>
     </row>
     <row r="251">
-      <c r="A251" s="155"/>
+      <c r="A251" s="159"/>
       <c r="G251" s="29"/>
       <c r="H251" s="29"/>
     </row>
     <row r="252">
-      <c r="A252" s="155"/>
+      <c r="A252" s="159"/>
       <c r="G252" s="29"/>
       <c r="H252" s="29"/>
     </row>
     <row r="253">
-      <c r="A253" s="155"/>
+      <c r="A253" s="159"/>
       <c r="G253" s="29"/>
       <c r="H253" s="29"/>
     </row>
     <row r="254">
-      <c r="A254" s="155"/>
+      <c r="A254" s="159"/>
       <c r="G254" s="29"/>
       <c r="H254" s="29"/>
     </row>
     <row r="255">
-      <c r="A255" s="155"/>
+      <c r="A255" s="159"/>
       <c r="G255" s="29"/>
       <c r="H255" s="29"/>
     </row>
     <row r="256">
-      <c r="A256" s="155"/>
+      <c r="A256" s="159"/>
       <c r="G256" s="29"/>
       <c r="H256" s="29"/>
     </row>
     <row r="257">
-      <c r="A257" s="155"/>
+      <c r="A257" s="159"/>
       <c r="G257" s="29"/>
       <c r="H257" s="29"/>
     </row>
     <row r="258">
-      <c r="A258" s="155"/>
+      <c r="A258" s="159"/>
       <c r="G258" s="29"/>
       <c r="H258" s="29"/>
     </row>
     <row r="259">
-      <c r="A259" s="155"/>
+      <c r="A259" s="159"/>
       <c r="G259" s="29"/>
       <c r="H259" s="29"/>
     </row>
     <row r="260">
-      <c r="A260" s="155"/>
+      <c r="A260" s="159"/>
       <c r="G260" s="29"/>
       <c r="H260" s="29"/>
     </row>
     <row r="261">
-      <c r="A261" s="155"/>
+      <c r="A261" s="159"/>
       <c r="G261" s="29"/>
       <c r="H261" s="29"/>
     </row>
     <row r="262">
-      <c r="A262" s="155"/>
+      <c r="A262" s="159"/>
       <c r="G262" s="29"/>
       <c r="H262" s="29"/>
     </row>
     <row r="263">
-      <c r="A263" s="155"/>
+      <c r="A263" s="159"/>
       <c r="G263" s="29"/>
       <c r="H263" s="29"/>
     </row>
     <row r="264">
-      <c r="A264" s="155"/>
+      <c r="A264" s="159"/>
       <c r="G264" s="29"/>
       <c r="H264" s="29"/>
     </row>
     <row r="265">
-      <c r="A265" s="155"/>
+      <c r="A265" s="159"/>
       <c r="G265" s="29"/>
       <c r="H265" s="29"/>
     </row>
     <row r="266">
-      <c r="A266" s="155"/>
+      <c r="A266" s="159"/>
       <c r="G266" s="29"/>
       <c r="H266" s="29"/>
     </row>
     <row r="267">
-      <c r="A267" s="155"/>
+      <c r="A267" s="159"/>
       <c r="G267" s="29"/>
       <c r="H267" s="29"/>
     </row>
     <row r="268">
-      <c r="A268" s="155"/>
+      <c r="A268" s="159"/>
       <c r="G268" s="29"/>
       <c r="H268" s="29"/>
     </row>
     <row r="269">
-      <c r="A269" s="155"/>
+      <c r="A269" s="159"/>
       <c r="G269" s="29"/>
       <c r="H269" s="29"/>
     </row>
     <row r="270">
-      <c r="A270" s="155"/>
+      <c r="A270" s="159"/>
       <c r="G270" s="29"/>
       <c r="H270" s="29"/>
     </row>
     <row r="271">
-      <c r="A271" s="155"/>
+      <c r="A271" s="159"/>
       <c r="G271" s="29"/>
       <c r="H271" s="29"/>
     </row>
     <row r="272">
-      <c r="A272" s="155"/>
+      <c r="A272" s="159"/>
       <c r="G272" s="29"/>
       <c r="H272" s="29"/>
     </row>
     <row r="273">
-      <c r="A273" s="155"/>
+      <c r="A273" s="159"/>
       <c r="G273" s="29"/>
       <c r="H273" s="29"/>
     </row>
     <row r="274">
-      <c r="A274" s="155"/>
+      <c r="A274" s="159"/>
       <c r="G274" s="29"/>
       <c r="H274" s="29"/>
     </row>
     <row r="275">
-      <c r="A275" s="155"/>
+      <c r="A275" s="159"/>
       <c r="G275" s="29"/>
       <c r="H275" s="29"/>
     </row>
     <row r="276">
-      <c r="A276" s="155"/>
+      <c r="A276" s="159"/>
       <c r="G276" s="29"/>
       <c r="H276" s="29"/>
     </row>
     <row r="277">
-      <c r="A277" s="155"/>
+      <c r="A277" s="159"/>
       <c r="G277" s="29"/>
       <c r="H277" s="29"/>
     </row>
     <row r="278">
-      <c r="A278" s="155"/>
+      <c r="A278" s="159"/>
       <c r="G278" s="29"/>
       <c r="H278" s="29"/>
     </row>
     <row r="279">
-      <c r="A279" s="155"/>
+      <c r="A279" s="159"/>
       <c r="G279" s="29"/>
       <c r="H279" s="29"/>
     </row>
     <row r="280">
-      <c r="A280" s="155"/>
+      <c r="A280" s="159"/>
       <c r="G280" s="29"/>
       <c r="H280" s="29"/>
     </row>
     <row r="281">
-      <c r="A281" s="155"/>
+      <c r="A281" s="159"/>
       <c r="G281" s="29"/>
       <c r="H281" s="29"/>
     </row>
     <row r="282">
-      <c r="A282" s="155"/>
+      <c r="A282" s="159"/>
       <c r="G282" s="29"/>
       <c r="H282" s="29"/>
     </row>
     <row r="283">
-      <c r="A283" s="155"/>
+      <c r="A283" s="159"/>
       <c r="G283" s="29"/>
       <c r="H283" s="29"/>
     </row>
     <row r="284">
-      <c r="A284" s="155"/>
+      <c r="A284" s="159"/>
       <c r="G284" s="29"/>
       <c r="H284" s="29"/>
     </row>
     <row r="285">
-      <c r="A285" s="155"/>
+      <c r="A285" s="159"/>
       <c r="G285" s="29"/>
       <c r="H285" s="29"/>
     </row>
     <row r="286">
-      <c r="A286" s="155"/>
+      <c r="A286" s="159"/>
       <c r="G286" s="29"/>
       <c r="H286" s="29"/>
     </row>
     <row r="287">
-      <c r="A287" s="155"/>
+      <c r="A287" s="159"/>
       <c r="G287" s="29"/>
       <c r="H287" s="29"/>
     </row>
     <row r="288">
-      <c r="A288" s="155"/>
+      <c r="A288" s="159"/>
       <c r="G288" s="29"/>
       <c r="H288" s="29"/>
     </row>
     <row r="289">
-      <c r="A289" s="155"/>
+      <c r="A289" s="159"/>
       <c r="G289" s="29"/>
       <c r="H289" s="29"/>
     </row>
     <row r="290">
-      <c r="A290" s="155"/>
+      <c r="A290" s="159"/>
       <c r="G290" s="29"/>
       <c r="H290" s="29"/>
     </row>
     <row r="291">
-      <c r="A291" s="155"/>
+      <c r="A291" s="159"/>
       <c r="G291" s="29"/>
       <c r="H291" s="29"/>
     </row>
     <row r="292">
-      <c r="A292" s="155"/>
+      <c r="A292" s="159"/>
       <c r="G292" s="29"/>
       <c r="H292" s="29"/>
     </row>
     <row r="293">
-      <c r="A293" s="155"/>
+      <c r="A293" s="159"/>
       <c r="G293" s="29"/>
       <c r="H293" s="29"/>
     </row>
     <row r="294">
-      <c r="A294" s="155"/>
+      <c r="A294" s="159"/>
       <c r="G294" s="29"/>
       <c r="H294" s="29"/>
     </row>
     <row r="295">
-      <c r="A295" s="155"/>
+      <c r="A295" s="159"/>
       <c r="G295" s="29"/>
       <c r="H295" s="29"/>
     </row>
     <row r="296">
-      <c r="A296" s="155"/>
+      <c r="A296" s="159"/>
       <c r="G296" s="29"/>
       <c r="H296" s="29"/>
     </row>
     <row r="297">
-      <c r="A297" s="155"/>
+      <c r="A297" s="159"/>
       <c r="G297" s="29"/>
       <c r="H297" s="29"/>
     </row>
     <row r="298">
-      <c r="A298" s="155"/>
+      <c r="A298" s="159"/>
       <c r="G298" s="29"/>
       <c r="H298" s="29"/>
     </row>
     <row r="299">
-      <c r="A299" s="155"/>
+      <c r="A299" s="159"/>
       <c r="G299" s="29"/>
       <c r="H299" s="29"/>
     </row>
     <row r="300">
-      <c r="A300" s="155"/>
+      <c r="A300" s="159"/>
       <c r="G300" s="29"/>
       <c r="H300" s="29"/>
     </row>
     <row r="301">
-      <c r="A301" s="155"/>
+      <c r="A301" s="159"/>
       <c r="G301" s="29"/>
       <c r="H301" s="29"/>
     </row>
     <row r="302">
-      <c r="A302" s="155"/>
+      <c r="A302" s="159"/>
       <c r="G302" s="29"/>
       <c r="H302" s="29"/>
     </row>
     <row r="303">
-      <c r="A303" s="155"/>
+      <c r="A303" s="159"/>
       <c r="G303" s="29"/>
       <c r="H303" s="29"/>
     </row>
     <row r="304">
-      <c r="A304" s="155"/>
+      <c r="A304" s="159"/>
       <c r="G304" s="29"/>
       <c r="H304" s="29"/>
     </row>
     <row r="305">
-      <c r="A305" s="155"/>
+      <c r="A305" s="159"/>
       <c r="G305" s="29"/>
       <c r="H305" s="29"/>
     </row>
@@ -18648,27 +18673,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="157" t="s">
+      <c r="C1" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="157" t="s">
+      <c r="D1" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="157" t="s">
+      <c r="E1" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="157" t="s">
+      <c r="F1" s="161" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="79" t="s">
         <v>952</v>
       </c>
       <c r="B2" s="51" t="s">
@@ -18686,10 +18711,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="79" t="s">
         <v>952</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>953</v>
       </c>
       <c r="C3" s="74" t="s">
@@ -18704,62 +18729,62 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="158" t="s">
+      <c r="A4" s="162" t="s">
         <v>252</v>
       </c>
       <c r="B4" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
       <c r="E4" s="42" t="s">
         <v>959</v>
       </c>
-      <c r="F4" s="111" t="s">
+      <c r="F4" s="115" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="162" t="s">
         <v>327</v>
       </c>
       <c r="B5" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
       <c r="E5" s="42" t="s">
         <v>961</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>962</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="159"/>
-      <c r="Z5" s="159"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
+      <c r="O5" s="163"/>
+      <c r="P5" s="163"/>
+      <c r="Q5" s="163"/>
+      <c r="R5" s="163"/>
+      <c r="S5" s="163"/>
+      <c r="T5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
+      <c r="X5" s="163"/>
+      <c r="Y5" s="163"/>
+      <c r="Z5" s="163"/>
     </row>
     <row r="6">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="79" t="s">
         <v>963</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="78" t="s">
         <v>964</v>
       </c>
       <c r="C6" s="74" t="s">
@@ -18774,29 +18799,29 @@
       <c r="F6" s="51" t="s">
         <v>968</v>
       </c>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159"/>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="159"/>
-      <c r="O6" s="159"/>
-      <c r="P6" s="159"/>
-      <c r="Q6" s="159"/>
-      <c r="R6" s="159"/>
-      <c r="S6" s="159"/>
-      <c r="T6" s="159"/>
-      <c r="U6" s="159"/>
-      <c r="V6" s="159"/>
-      <c r="W6" s="159"/>
-      <c r="X6" s="159"/>
-      <c r="Y6" s="159"/>
-      <c r="Z6" s="159"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
+      <c r="M6" s="163"/>
+      <c r="N6" s="163"/>
+      <c r="O6" s="163"/>
+      <c r="P6" s="163"/>
+      <c r="Q6" s="163"/>
+      <c r="R6" s="163"/>
+      <c r="S6" s="163"/>
+      <c r="T6" s="163"/>
+      <c r="U6" s="163"/>
+      <c r="V6" s="163"/>
+      <c r="W6" s="163"/>
+      <c r="X6" s="163"/>
+      <c r="Y6" s="163"/>
+      <c r="Z6" s="163"/>
     </row>
     <row r="7">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="79" t="s">
         <v>526</v>
       </c>
       <c r="B7" s="51" t="s">
@@ -18819,65 +18844,65 @@
       <c r="A8" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="78" t="s">
         <v>605</v>
       </c>
-      <c r="C8" s="160" t="s">
+      <c r="C8" s="164" t="s">
         <v>606</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="78" t="s">
         <v>970</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="78" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="158" t="s">
+      <c r="A9" s="162" t="s">
         <v>577</v>
       </c>
       <c r="B9" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
       <c r="E9" s="68" t="s">
         <v>972</v>
       </c>
-      <c r="F9" s="161" t="s">
+      <c r="F9" s="165" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="162" t="s">
         <v>577</v>
       </c>
       <c r="B10" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
       <c r="E10" s="68" t="s">
         <v>972</v>
       </c>
-      <c r="F10" s="161" t="s">
+      <c r="F10" s="165" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="104" t="s">
         <v>610</v>
       </c>
       <c r="B11" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
       <c r="E11" s="68" t="s">
         <v>975</v>
       </c>
-      <c r="F11" s="161" t="s">
+      <c r="F11" s="165" t="s">
         <v>976</v>
       </c>
     </row>
@@ -18885,7 +18910,7 @@
       <c r="A12" s="6" t="s">
         <v>650</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="78" t="s">
         <v>651</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -18894,22 +18919,22 @@
       <c r="D12" s="6" t="s">
         <v>653</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="78" t="s">
         <v>977</v>
       </c>
-      <c r="F12" s="77" t="s">
+      <c r="F12" s="78" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="104" t="s">
         <v>661</v>
       </c>
       <c r="B13" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
       <c r="E13" s="68" t="s">
         <v>979</v>
       </c>
@@ -22894,7 +22919,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="166" t="s">
         <v>981</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -22902,7 +22927,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="167" t="s">
         <v>983</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -22910,12 +22935,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="168" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="165" t="s">
+      <c r="A6" s="169" t="s">
         <v>986</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -22934,53 +22959,53 @@
       <c r="B9" s="21"/>
     </row>
     <row r="10">
-      <c r="A10" s="165" t="s">
+      <c r="A10" s="169" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="165" t="s">
+      <c r="A11" s="169" t="s">
         <v>990</v>
       </c>
-      <c r="B11" s="166" t="s">
+      <c r="B11" s="170" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="167" t="s">
+      <c r="B12" s="171" t="s">
         <v>992</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="168"/>
-      <c r="B13" s="169" t="s">
+      <c r="A13" s="172"/>
+      <c r="B13" s="173" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="170" t="s">
+      <c r="B14" s="174" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="175" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="172" t="s">
+      <c r="B16" s="176" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="165"/>
+      <c r="A17" s="169"/>
       <c r="B17" s="29"/>
     </row>
     <row r="18">
-      <c r="A18" s="165" t="s">
+      <c r="A18" s="169" t="s">
         <v>997</v>
       </c>
-      <c r="B18" s="173" t="s">
+      <c r="B18" s="177" t="s">
         <v>998</v>
       </c>
     </row>
@@ -22988,13 +23013,13 @@
       <c r="A19" s="6" t="s">
         <v>999</v>
       </c>
-      <c r="B19" s="174"/>
+      <c r="B19" s="178"/>
     </row>
     <row r="21">
-      <c r="A21" s="165" t="s">
+      <c r="A21" s="169" t="s">
         <v>1000</v>
       </c>
-      <c r="B21" s="175" t="s">
+      <c r="B21" s="179" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -23020,7 +23045,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="169" t="s">
         <v>1002</v>
       </c>
     </row>
@@ -23099,7 +23124,7 @@
       <c r="A1" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="180" t="s">
         <v>1013</v>
       </c>
     </row>
@@ -23167,7 +23192,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="166"/>
+      <c r="A1" s="170"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -23191,47 +23216,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="181" t="s">
         <v>1024</v>
       </c>
-      <c r="C1" s="177" t="s">
+      <c r="C1" s="181" t="s">
         <v>1025</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="169" t="s">
         <v>1026</v>
       </c>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>1027</v>
       </c>
-      <c r="C2" s="165" t="s">
+      <c r="C2" s="169" t="s">
         <v>1028</v>
       </c>
-      <c r="D2" s="165" t="s">
+      <c r="D2" s="169" t="s">
         <v>1029</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="178" t="s">
+      <c r="A3" s="182" t="s">
         <v>1030</v>
       </c>
-      <c r="B3" s="178" t="s">
+      <c r="B3" s="182" t="s">
         <v>1031</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="D3" s="179" t="str">
+      <c r="D3" s="183" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
         <v>ADDRESS_CONTRACTING_BODY</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="182" t="s">
         <v>1033</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="182" t="s">
         <v>1031</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -23243,10 +23268,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="166" t="s">
+      <c r="A5" s="170" t="s">
         <v>1034</v>
       </c>
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="170" t="s">
         <v>1035</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -23254,10 +23279,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="170" t="s">
         <v>1036</v>
       </c>
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="170" t="s">
         <v>1037</v>
       </c>
       <c r="C6" s="21" t="s">
@@ -23274,7 +23299,7 @@
       <c r="C7" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="D7" s="180" t="s">
+      <c r="D7" s="184" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -23288,7 +23313,7 @@
       <c r="C8" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="D8" s="181" t="s">
+      <c r="D8" s="185" t="s">
         <v>1043</v>
       </c>
     </row>
@@ -23332,21 +23357,21 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="181" t="s">
         <v>1024</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="169" t="s">
         <v>1026</v>
       </c>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>1027</v>
       </c>
-      <c r="C2" s="165" t="s">
+      <c r="C2" s="169" t="s">
         <v>1028</v>
       </c>
-      <c r="D2" s="165" t="s">
+      <c r="D2" s="169" t="s">
         <v>1029</v>
       </c>
     </row>
@@ -23373,7 +23398,7 @@
       <c r="B5" s="21" t="s">
         <v>1052</v>
       </c>
-      <c r="C5" s="181" t="s">
+      <c r="C5" s="185" t="s">
         <v>1050</v>
       </c>
       <c r="D5" s="21" t="s">

</xml_diff>

<commit_message>
Fixed module names for section 3 and confidentiality, both in CM v.6.1.1 and in the source TM.
</commit_message>
<xml_diff>
--- a/mappings/package_F06/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F06/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.1.0</t>
+    <t>6.1.1</t>
   </si>
   <si>
     <r>
@@ -7251,7 +7251,7 @@
     <t>notice.rml.ttl</t>
   </si>
   <si>
-    <t>confidentiality.ttl</t>
+    <t>confidentiality.rml.ttl</t>
   </si>
   <si>
     <t>Informal (if possible to become formal)</t>
@@ -8248,7 +8248,7 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="16" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>

</xml_diff>